<commit_message>
Dodana pliki z grafiką oraz stronę webową
</commit_message>
<xml_diff>
--- a/Jakub_Example.xlsx
+++ b/Jakub_Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\Projekt na zaliczenie\ALK_Python_Ed1_2023-2024_Jakub_M_Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9D60E74-653D-4D08-A865-5876F07E0773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D657751E-4935-47B2-A06A-EE7C774ADD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{37C0F546-9220-48F0-936F-3BE554F90A52}"/>
   </bookViews>
@@ -4103,10 +4103,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D226E1-FC1A-48F0-AD88-C0DA90581EDE}">
   <dimension ref="A1:AC16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" zoomScaleSheetLayoutView="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="87" zoomScaleNormal="87" zoomScaleSheetLayoutView="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomLeft" activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5198,7 +5198,7 @@
         <v>20</v>
       </c>
       <c r="T11" s="18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="U11" s="18" t="s">
         <v>20</v>
@@ -5299,7 +5299,7 @@
         <v>20</v>
       </c>
       <c r="T12" s="18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="U12" s="18" t="s">
         <v>20</v>
@@ -5400,7 +5400,7 @@
         <v>20</v>
       </c>
       <c r="T13" s="18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="U13" s="18" t="s">
         <v>20</v>
@@ -5501,7 +5501,7 @@
         <v>20</v>
       </c>
       <c r="T14" s="18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="U14" s="18" t="s">
         <v>20</v>
@@ -5602,7 +5602,7 @@
         <v>20</v>
       </c>
       <c r="T15" s="18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="U15" s="18" t="s">
         <v>20</v>
@@ -9865,21 +9865,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D124FEFF57024A4AA077731EED7D9DC1" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="006ca74950da2153477e534e4a5b6b65">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8c5ef8ea-0146-47b4-a56e-851ac557f1f2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="60aa03a645557395d9d3c3b3574fc504" ns2:_="">
     <xsd:import namespace="8c5ef8ea-0146-47b4-a56e-851ac557f1f2"/>
@@ -10023,10 +10008,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89ADE1A5-12BD-4A49-ADEF-14C62668174E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8FF241B-460E-4B46-8F17-F6D660217C72}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8c5ef8ea-0146-47b4-a56e-851ac557f1f2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10048,19 +10058,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8FF241B-460E-4B46-8F17-F6D660217C72}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89ADE1A5-12BD-4A49-ADEF-14C62668174E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8c5ef8ea-0146-47b4-a56e-851ac557f1f2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>